<commit_message>
Columna con tipo de biopsia, hoja con informes patológicos
</commit_message>
<xml_diff>
--- a/data/extras/ihc_slides/HER2.xlsx
+++ b/data/extras/ihc_slides/HER2.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Información original" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Información anotaciones" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Cruce patólogos" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Informes anatomo patológicos" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="400">
   <si>
     <t xml:space="preserve">Nombre Imagen</t>
   </si>
@@ -1107,7 +1108,10 @@
     <t xml:space="preserve">ID Paciente</t>
   </si>
   <si>
-    <t xml:space="preserve">Patólogo 0 (evaluación original)</t>
+    <t xml:space="preserve">Tipo de biopsia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patólogo 0</t>
   </si>
   <si>
     <t xml:space="preserve">Patólogo 1</t>
@@ -1119,15 +1123,15 @@
     <t xml:space="preserve">Evaluación final (consenso)</t>
   </si>
   <si>
-    <t xml:space="preserve">Descargada?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sí</t>
+    <t xml:space="preserve">Resección</t>
   </si>
   <si>
     <t xml:space="preserve">Escala de colores:</t>
   </si>
   <si>
+    <t xml:space="preserve">Endoscopia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tres patólogos coinciden </t>
   </si>
   <si>
@@ -1146,7 +1150,229 @@
     <t xml:space="preserve">Sólo 1 patólogo evalúa </t>
   </si>
   <si>
-    <t xml:space="preserve">No</t>
+    <t xml:space="preserve">ID Biopsia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID informe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre slide en ndp.microscopiavirtual.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-01 FGV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">252.309 LLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-08908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-02 CSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-08896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-04 RSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-00470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-06 LCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-03023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3995-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-07 FSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-03043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-08 CDV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-03237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-09 FAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">260.121 CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-03772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-10 MBN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-11 MES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-04358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-12 LOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-04873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID informe no coincide con ID biopsia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-13 CHV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011-5410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-15 OGP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-06076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1168-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-16 OAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">269.141 GCLIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-07164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-17 LMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">266.437 CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-06894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-18 CQV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-00381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-07429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-19 HVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-08046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-22 APY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-08890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-24 LRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No había informe patológico en la carpeta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-26 AGC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011-1217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-27 PBM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-30 LAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-10345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-10224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-35 JJM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-36 BCG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-36 BLG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-37 HCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-38 APA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-39 SBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-40 MRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-43 MFM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-46 CRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-48 NCV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-50 MVG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-52 ARP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-53 PLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-54 LCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-55 LCN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-56 TCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-57 RUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-57 RVM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-59 SMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-60 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-01-61 MCT</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1383,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1236,8 +1462,37 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1271,7 +1526,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA40000"/>
-        <bgColor rgb="FF840000"/>
+        <bgColor rgb="FFB00000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1325,13 +1580,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC46200"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFC4A000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7F7F7F"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB00000"/>
+        <bgColor rgb="FFA40000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1490,15 +1751,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1506,15 +1763,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1530,11 +1783,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1562,62 +1815,70 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1673,7 +1934,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF005800"/>
       <rgbColor rgb="FF264F05"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFB00000"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF204A87"/>
       <rgbColor rgb="FF333333"/>
@@ -1689,8 +1950,8 @@
   </sheetPr>
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2607,8 +2868,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2620,7 +2881,7 @@
   </sheetPr>
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -6893,8 +7154,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6904,25 +7165,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="39.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="27.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="14.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="36.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="25.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="28" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="28" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="51.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6935,16 +7196,16 @@
       <c r="C1" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="2" t="s">
         <v>312</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="29" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6955,289 +7216,290 @@
       <c r="B2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="C2" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="D2" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="36" t="n">
+      <c r="C3" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D3" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="F3" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>316</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="39" t="s">
+      <c r="D5" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="42" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="33" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="42" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="s">
+      <c r="D6" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="43" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="33" t="s">
         <v>316</v>
       </c>
-      <c r="J4" s="43" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="42" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="D10" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="33" t="s">
         <v>316</v>
       </c>
-      <c r="J5" s="44" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="0" t="s">
+      <c r="D11" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="40" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="36"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="33" t="s">
         <v>316</v>
       </c>
-      <c r="J6" s="45" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="J7" s="46" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="J8" s="47" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="F9" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="C11" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="41" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" s="42" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="36" t="n">
+      <c r="D13" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="E13" s="36" t="n">
+      <c r="F13" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="F13" s="37" t="n">
+      <c r="G13" s="35" t="n">
         <v>3</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7247,20 +7509,20 @@
       <c r="B14" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="31" t="n">
+      <c r="C14" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="D14" s="32" t="n">
+      <c r="E14" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="E14" s="32" t="n">
+      <c r="F14" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="33" t="n">
+      <c r="G14" s="32" t="n">
         <v>3</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7270,752 +7532,1885 @@
       <c r="B15" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="31" t="n">
+      <c r="C15" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="D15" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="32" t="n">
+      <c r="E15" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="E15" s="32" t="n">
+      <c r="F15" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="33" t="n">
+      <c r="G15" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="38" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="41" t="n">
+      <c r="D16" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25" t="n">
+      <c r="E16" s="39"/>
+      <c r="F16" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="F16" s="42" t="n">
+      <c r="G16" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="38" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="41" t="n">
+      <c r="D17" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25" t="n">
+      <c r="E17" s="39"/>
+      <c r="F17" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="F17" s="42" t="n">
+      <c r="G17" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="G17" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="38" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="41" t="n">
+      <c r="D18" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25" t="n">
+      <c r="E18" s="39"/>
+      <c r="F18" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="F18" s="42" t="n">
+      <c r="G18" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>316</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="50" t="n">
+      <c r="C19" s="46"/>
+      <c r="D19" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="F19" s="51"/>
+      <c r="F19" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54" t="n">
+      <c r="C20" s="49"/>
+      <c r="D20" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="55"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54" t="n">
+      <c r="C21" s="49"/>
+      <c r="D21" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="55"/>
+      <c r="G21" s="51"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C22" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54" t="n">
+      <c r="C22" s="49"/>
+      <c r="D22" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="55"/>
+      <c r="G22" s="51"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F23" s="55"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="51"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="52" t="s">
+      <c r="A24" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F24" s="55"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="51"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F25" s="55"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="51"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="52" t="s">
+      <c r="B26" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F26" s="55"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="51"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F27" s="55"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="51"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="52" t="s">
+      <c r="A28" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F28" s="55"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="51"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="52" t="s">
+      <c r="A29" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F29" s="55"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" s="51"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F30" s="55"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="51"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="52" t="s">
+      <c r="B31" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="C31" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F31" s="55"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="51"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F32" s="55"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="51"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F33" s="55"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="51"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="52" t="s">
+      <c r="A34" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="52" t="s">
+      <c r="B34" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F34" s="55"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" s="51"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="52" t="s">
+      <c r="A35" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="53" t="n">
+      <c r="C35" s="49"/>
+      <c r="D35" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F35" s="55"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" s="51"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="53" t="n">
+      <c r="C36" s="49"/>
+      <c r="D36" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F36" s="55"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" s="51"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="52" t="s">
+      <c r="A37" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="53" t="n">
+      <c r="C37" s="49"/>
+      <c r="D37" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F37" s="55"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" s="51"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="53" t="n">
+      <c r="C38" s="49"/>
+      <c r="D38" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="F38" s="55"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" s="51"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="52" t="s">
+      <c r="B39" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="53" t="n">
+      <c r="C39" s="49"/>
+      <c r="D39" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54" t="n">
+      <c r="E39" s="50"/>
+      <c r="F39" s="50" t="n">
         <v>3</v>
       </c>
-      <c r="F39" s="55"/>
+      <c r="G39" s="51"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="59"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="54"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="56" t="s">
+      <c r="A41" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="59"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="54"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="59"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="54"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="59"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="54"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="56" t="s">
+      <c r="A44" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="59"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="54"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="56" t="s">
+      <c r="A45" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="56" t="s">
+      <c r="B45" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="59"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="54"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="59"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="54"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="56" t="s">
+      <c r="A47" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="59"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="54"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="56" t="s">
+      <c r="A48" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="59"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="54"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="59"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="54"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="56" t="s">
+      <c r="A50" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="56" t="s">
+      <c r="B50" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="59"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="54"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="56" t="s">
+      <c r="A51" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="56" t="s">
+      <c r="B51" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="59"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="54"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="59"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="54"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="56" t="s">
+      <c r="A53" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="56" t="s">
+      <c r="B53" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="C53" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="59"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="54"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="56" t="s">
+      <c r="A54" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="56" t="s">
+      <c r="B54" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C54" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="59"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="54"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="59"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="54"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="56" t="s">
+      <c r="A56" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="B56" s="56" t="s">
+      <c r="B56" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C56" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" s="58"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="59"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="54"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="B57" s="56" t="s">
+      <c r="B57" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="C57" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="59"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="54"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="56" t="s">
+      <c r="A58" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="56" t="s">
+      <c r="B58" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="C58" s="57" t="n">
+      <c r="C58" s="52"/>
+      <c r="D58" s="53" t="n">
         <v>1</v>
       </c>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="59"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="54"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="56" t="s">
+      <c r="A59" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="B59" s="56" t="s">
+      <c r="B59" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C59" s="57" t="n">
+      <c r="C59" s="52"/>
+      <c r="D59" s="53" t="n">
         <v>1</v>
       </c>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
-      <c r="F59" s="59"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="54"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="56" t="s">
+      <c r="A60" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="B60" s="56" t="s">
+      <c r="B60" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="57" t="n">
+      <c r="C60" s="52"/>
+      <c r="D60" s="53" t="n">
         <v>1</v>
       </c>
-      <c r="D60" s="58"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="59"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="53"/>
+      <c r="G60" s="54"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="56" t="s">
+      <c r="A61" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="B61" s="56" t="s">
+      <c r="B61" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C61" s="57" t="n">
-        <v>2</v>
-      </c>
-      <c r="D61" s="58"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="59"/>
+      <c r="C61" s="52"/>
+      <c r="D61" s="53" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="54"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="56" t="s">
+      <c r="A62" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B62" s="56" t="s">
+      <c r="B62" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="C62" s="57" t="n">
+      <c r="C62" s="52"/>
+      <c r="D62" s="53" t="n">
         <v>3</v>
       </c>
-      <c r="D62" s="58"/>
-      <c r="E62" s="58"/>
-      <c r="F62" s="59"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="53"/>
+      <c r="G62" s="54"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G62"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="55" width="27.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="55" width="33.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="55" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="55" width="28.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="55" width="37.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="55" width="50.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="55" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="43.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="56" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>325</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>326</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="57" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>330</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="57"/>
+      <c r="G2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="57" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="57"/>
+      <c r="G3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="57" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="57"/>
+      <c r="G4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="57" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>335</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="57"/>
+      <c r="G5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" s="57" t="s">
+        <v>337</v>
+      </c>
+      <c r="E6" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="57"/>
+      <c r="G6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>338</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="57"/>
+      <c r="G7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="57" t="s">
+        <v>339</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="57"/>
+      <c r="G8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>342</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="57"/>
+      <c r="G9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="57" t="s">
+        <v>343</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="57"/>
+      <c r="G10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="57" t="s">
+        <v>343</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D11" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="57"/>
+      <c r="G11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" s="57" t="n">
+        <v>102974</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="57"/>
+      <c r="G12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="57"/>
+      <c r="G13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="58" t="s">
+        <v>349</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" s="58" t="s">
+        <v>350</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="58" t="s">
+        <v>351</v>
+      </c>
+      <c r="G14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="57"/>
+      <c r="G15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="E16" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="57"/>
+      <c r="G16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="D17" s="57" t="s">
+        <v>356</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="57"/>
+      <c r="G17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="57" t="s">
+        <v>357</v>
+      </c>
+      <c r="B18" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>358</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="57"/>
+      <c r="G18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="57" t="s">
+        <v>357</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>359</v>
+      </c>
+      <c r="E19" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="57"/>
+      <c r="G19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="E20" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="57"/>
+      <c r="G20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>362</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="57"/>
+      <c r="G21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="58" t="s">
+        <v>363</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="58" t="s">
+        <v>318</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>364</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>351</v>
+      </c>
+      <c r="G22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>365</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="57"/>
+      <c r="G23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="57" t="s">
+        <v>366</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>367</v>
+      </c>
+      <c r="E24" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="57"/>
+      <c r="G24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="57" t="s">
+        <v>368</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>369</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="57"/>
+      <c r="G25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="59" t="s">
+        <v>370</v>
+      </c>
+      <c r="B26" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="59" t="s">
+        <v>371</v>
+      </c>
+      <c r="G26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="57" t="s">
+        <v>372</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>373</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="57"/>
+      <c r="G27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="59" t="s">
+        <v>374</v>
+      </c>
+      <c r="B28" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="59" t="s">
+        <v>371</v>
+      </c>
+      <c r="G28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="58" t="s">
+        <v>375</v>
+      </c>
+      <c r="B29" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="58" t="s">
+        <v>316</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>376</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" s="58" t="s">
+        <v>351</v>
+      </c>
+      <c r="G29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="58" t="s">
+        <v>375</v>
+      </c>
+      <c r="B30" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="58" t="s">
+        <v>318</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>377</v>
+      </c>
+      <c r="E30" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="58" t="s">
+        <v>351</v>
+      </c>
+      <c r="G30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="59" t="s">
+        <v>378</v>
+      </c>
+      <c r="B31" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="59"/>
+      <c r="G31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="59" t="s">
+        <v>378</v>
+      </c>
+      <c r="B32" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="59"/>
+      <c r="G32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="59" t="s">
+        <v>379</v>
+      </c>
+      <c r="B33" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="59"/>
+      <c r="G33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="59" t="s">
+        <v>380</v>
+      </c>
+      <c r="B34" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" s="59"/>
+      <c r="G34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="59" t="s">
+        <v>381</v>
+      </c>
+      <c r="B35" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="59"/>
+      <c r="G35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="59" t="s">
+        <v>381</v>
+      </c>
+      <c r="B36" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="59"/>
+      <c r="G36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="59" t="s">
+        <v>382</v>
+      </c>
+      <c r="B37" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" s="59"/>
+      <c r="G37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="59" t="s">
+        <v>383</v>
+      </c>
+      <c r="B38" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="59"/>
+      <c r="G38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="59" t="s">
+        <v>383</v>
+      </c>
+      <c r="B39" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="59"/>
+      <c r="G39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="59" t="s">
+        <v>384</v>
+      </c>
+      <c r="B40" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="59"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="F40" s="59"/>
+      <c r="G40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="59" t="s">
+        <v>385</v>
+      </c>
+      <c r="B41" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="F41" s="59"/>
+      <c r="G41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="59" t="s">
+        <v>386</v>
+      </c>
+      <c r="B42" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" s="59"/>
+      <c r="G42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="59" t="s">
+        <v>386</v>
+      </c>
+      <c r="B43" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" s="59"/>
+      <c r="G43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="59" t="s">
+        <v>387</v>
+      </c>
+      <c r="B44" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" s="59"/>
+      <c r="G44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="59" t="s">
+        <v>387</v>
+      </c>
+      <c r="B45" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="F45" s="59"/>
+      <c r="G45" s="0"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="59" t="s">
+        <v>388</v>
+      </c>
+      <c r="B46" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="F46" s="59"/>
+      <c r="G46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="59" t="s">
+        <v>389</v>
+      </c>
+      <c r="B47" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="59"/>
+      <c r="G47" s="0"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="59" t="s">
+        <v>389</v>
+      </c>
+      <c r="B48" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="59"/>
+      <c r="G48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="59" t="s">
+        <v>390</v>
+      </c>
+      <c r="B49" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="59"/>
+      <c r="G49" s="0"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="59" t="s">
+        <v>390</v>
+      </c>
+      <c r="B50" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50" s="59"/>
+      <c r="G50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="59" t="s">
+        <v>391</v>
+      </c>
+      <c r="B51" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="59"/>
+      <c r="G51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="59" t="s">
+        <v>392</v>
+      </c>
+      <c r="B52" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52" s="59"/>
+      <c r="G52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="59" t="s">
+        <v>393</v>
+      </c>
+      <c r="B53" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="F53" s="59"/>
+      <c r="G53" s="0"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="59" t="s">
+        <v>393</v>
+      </c>
+      <c r="B54" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="59"/>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="59"/>
+      <c r="G54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="59" t="s">
+        <v>394</v>
+      </c>
+      <c r="B55" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="59"/>
+      <c r="G55" s="0"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="59" t="s">
+        <v>395</v>
+      </c>
+      <c r="B56" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" s="59"/>
+      <c r="G56" s="0"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="59" t="s">
+        <v>396</v>
+      </c>
+      <c r="B57" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="59"/>
+      <c r="G57" s="0"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="B58" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="59"/>
+      <c r="G58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="59" t="s">
+        <v>398</v>
+      </c>
+      <c r="B59" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="F59" s="59"/>
+      <c r="G59" s="0"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="59" t="s">
+        <v>399</v>
+      </c>
+      <c r="B60" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="F60" s="59"/>
+      <c r="G60" s="0"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="59" t="s">
+        <v>399</v>
+      </c>
+      <c r="B61" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="59"/>
+      <c r="G61" s="0"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="59" t="s">
+        <v>399</v>
+      </c>
+      <c r="B62" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="59"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" s="59"/>
+      <c r="G62" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Coordenadas donde empieza slide sin tejido control
</commit_message>
<xml_diff>
--- a/data/extras/ihc_slides/HER2.xlsx
+++ b/data/extras/ihc_slides/HER2.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Información original" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Información anotaciones" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Cruce patólogos" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Informes anatomo patológicos" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Asdf" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="408">
   <si>
     <t xml:space="preserve">Nombre Imagen</t>
   </si>
@@ -1373,6 +1374,30 @@
   </si>
   <si>
     <t xml:space="preserve">2009-01-61 MCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordenada X inicial (μm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordenada X inicial (pixeles)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># de resecciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># de endocopias</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># de resecciones con consenso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># de endocopias con consenso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o endoscopia?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O resección?</t>
   </si>
 </sst>
 </file>
@@ -1950,7 +1975,7 @@
   </sheetPr>
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2861,6 +2886,7 @@
       <c r="E67" s="17"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="1">
     <mergeCell ref="A28:E30"/>
   </mergeCells>
@@ -2882,7 +2908,7 @@
   <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7110,6 +7136,7 @@
       <c r="G201" s="25"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="38">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A13"/>
@@ -7167,13 +7194,13 @@
   </sheetPr>
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="36.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="36.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="25.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="28" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="14.88"/>
@@ -7618,7 +7645,9 @@
       <c r="B19" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="46"/>
+      <c r="C19" s="46" t="s">
+        <v>316</v>
+      </c>
       <c r="D19" s="47" t="n">
         <v>0</v>
       </c>
@@ -7637,7 +7666,9 @@
       <c r="B20" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D20" s="50" t="n">
         <v>0</v>
       </c>
@@ -7654,7 +7685,9 @@
       <c r="B21" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="49"/>
+      <c r="C21" s="49" t="s">
+        <v>318</v>
+      </c>
       <c r="D21" s="50" t="n">
         <v>0</v>
       </c>
@@ -7671,7 +7704,9 @@
       <c r="B22" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C22" s="49"/>
+      <c r="C22" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D22" s="50" t="n">
         <v>0</v>
       </c>
@@ -7688,7 +7723,9 @@
       <c r="B23" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="49"/>
+      <c r="C23" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D23" s="50" t="n">
         <v>0</v>
       </c>
@@ -7705,7 +7742,9 @@
       <c r="B24" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="49"/>
+      <c r="C24" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D24" s="50" t="n">
         <v>0</v>
       </c>
@@ -7722,7 +7761,9 @@
       <c r="B25" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D25" s="50" t="n">
         <v>0</v>
       </c>
@@ -7739,7 +7780,9 @@
       <c r="B26" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="49"/>
+      <c r="C26" s="49" t="s">
+        <v>318</v>
+      </c>
       <c r="D26" s="50" t="n">
         <v>0</v>
       </c>
@@ -7756,7 +7799,9 @@
       <c r="B27" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="49"/>
+      <c r="C27" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D27" s="50" t="n">
         <v>0</v>
       </c>
@@ -7773,7 +7818,9 @@
       <c r="B28" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="49"/>
+      <c r="C28" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D28" s="50" t="n">
         <v>0</v>
       </c>
@@ -7790,7 +7837,9 @@
       <c r="B29" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="49"/>
+      <c r="C29" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D29" s="50" t="n">
         <v>0</v>
       </c>
@@ -7807,7 +7856,9 @@
       <c r="B30" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="49"/>
+      <c r="C30" s="49" t="s">
+        <v>318</v>
+      </c>
       <c r="D30" s="50" t="n">
         <v>0</v>
       </c>
@@ -7824,7 +7875,9 @@
       <c r="B31" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="C31" s="49"/>
+      <c r="C31" s="49" t="s">
+        <v>318</v>
+      </c>
       <c r="D31" s="50" t="n">
         <v>0</v>
       </c>
@@ -7841,7 +7894,9 @@
       <c r="B32" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="49"/>
+      <c r="C32" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D32" s="50" t="n">
         <v>0</v>
       </c>
@@ -7858,7 +7913,9 @@
       <c r="B33" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="49"/>
+      <c r="C33" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D33" s="50" t="n">
         <v>0</v>
       </c>
@@ -7875,7 +7932,9 @@
       <c r="B34" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="49"/>
+      <c r="C34" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D34" s="50" t="n">
         <v>0</v>
       </c>
@@ -7892,7 +7951,9 @@
       <c r="B35" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="49"/>
+      <c r="C35" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D35" s="50" t="n">
         <v>1</v>
       </c>
@@ -7909,7 +7970,9 @@
       <c r="B36" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="49"/>
+      <c r="C36" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D36" s="50" t="n">
         <v>1</v>
       </c>
@@ -7926,7 +7989,9 @@
       <c r="B37" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="49"/>
+      <c r="C37" s="49" t="s">
+        <v>318</v>
+      </c>
       <c r="D37" s="50" t="n">
         <v>1</v>
       </c>
@@ -7943,7 +8008,9 @@
       <c r="B38" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="49"/>
+      <c r="C38" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D38" s="50" t="n">
         <v>1</v>
       </c>
@@ -7960,7 +8027,9 @@
       <c r="B39" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="49"/>
+      <c r="C39" s="49" t="s">
+        <v>316</v>
+      </c>
       <c r="D39" s="50" t="n">
         <v>1</v>
       </c>
@@ -7977,7 +8046,9 @@
       <c r="B40" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="52"/>
+      <c r="C40" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D40" s="53" t="n">
         <v>0</v>
       </c>
@@ -7992,7 +8063,9 @@
       <c r="B41" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="52"/>
+      <c r="C41" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D41" s="53" t="n">
         <v>0</v>
       </c>
@@ -8007,7 +8080,9 @@
       <c r="B42" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="52"/>
+      <c r="C42" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D42" s="53" t="n">
         <v>0</v>
       </c>
@@ -8022,7 +8097,9 @@
       <c r="B43" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="52"/>
+      <c r="C43" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D43" s="53" t="n">
         <v>0</v>
       </c>
@@ -8037,7 +8114,9 @@
       <c r="B44" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="52"/>
+      <c r="C44" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D44" s="53" t="n">
         <v>0</v>
       </c>
@@ -8052,7 +8131,9 @@
       <c r="B45" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="52"/>
+      <c r="C45" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D45" s="53" t="n">
         <v>0</v>
       </c>
@@ -8067,7 +8148,9 @@
       <c r="B46" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="52"/>
+      <c r="C46" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D46" s="53" t="n">
         <v>0</v>
       </c>
@@ -8082,7 +8165,9 @@
       <c r="B47" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="52"/>
+      <c r="C47" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D47" s="53" t="n">
         <v>0</v>
       </c>
@@ -8097,7 +8182,9 @@
       <c r="B48" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="52"/>
+      <c r="C48" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D48" s="53" t="n">
         <v>0</v>
       </c>
@@ -8112,7 +8199,9 @@
       <c r="B49" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="52"/>
+      <c r="C49" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D49" s="53" t="n">
         <v>0</v>
       </c>
@@ -8127,7 +8216,9 @@
       <c r="B50" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="52"/>
+      <c r="C50" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D50" s="53" t="n">
         <v>0</v>
       </c>
@@ -8142,7 +8233,9 @@
       <c r="B51" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="52"/>
+      <c r="C51" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D51" s="53" t="n">
         <v>0</v>
       </c>
@@ -8157,7 +8250,9 @@
       <c r="B52" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="52"/>
+      <c r="C52" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D52" s="53" t="n">
         <v>0</v>
       </c>
@@ -8172,7 +8267,9 @@
       <c r="B53" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="C53" s="52"/>
+      <c r="C53" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D53" s="53" t="n">
         <v>0</v>
       </c>
@@ -8187,7 +8284,9 @@
       <c r="B54" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C54" s="52"/>
+      <c r="C54" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D54" s="53" t="n">
         <v>0</v>
       </c>
@@ -8202,7 +8301,9 @@
       <c r="B55" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="52"/>
+      <c r="C55" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D55" s="53" t="n">
         <v>0</v>
       </c>
@@ -8217,7 +8318,9 @@
       <c r="B56" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C56" s="52"/>
+      <c r="C56" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D56" s="53" t="n">
         <v>0</v>
       </c>
@@ -8232,7 +8335,9 @@
       <c r="B57" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="C57" s="52"/>
+      <c r="C57" s="52" t="s">
+        <v>316</v>
+      </c>
       <c r="D57" s="53" t="n">
         <v>0</v>
       </c>
@@ -8247,7 +8352,9 @@
       <c r="B58" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="C58" s="52"/>
+      <c r="C58" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D58" s="53" t="n">
         <v>1</v>
       </c>
@@ -8262,7 +8369,9 @@
       <c r="B59" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C59" s="52"/>
+      <c r="C59" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D59" s="53" t="n">
         <v>1</v>
       </c>
@@ -8277,7 +8386,9 @@
       <c r="B60" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="52"/>
+      <c r="C60" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D60" s="53" t="n">
         <v>1</v>
       </c>
@@ -8292,7 +8403,9 @@
       <c r="B61" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C61" s="52"/>
+      <c r="C61" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D61" s="53" t="n">
         <v>2</v>
       </c>
@@ -8307,7 +8420,9 @@
       <c r="B62" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="C62" s="52"/>
+      <c r="C62" s="52" t="s">
+        <v>318</v>
+      </c>
       <c r="D62" s="53" t="n">
         <v>3</v>
       </c>
@@ -8316,6 +8431,7 @@
       <c r="G62" s="54"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -8334,15 +8450,15 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="55" width="27.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="55" width="27.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="55" width="33.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="55" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="55" width="28.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="55" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="55" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="55" width="50.6"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="55" width="11.52"/>
@@ -9403,6 +9519,1511 @@
       </c>
       <c r="F62" s="59"/>
       <c r="G62" s="0"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M62"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="33.46"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="28" width="2.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="14.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="16.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="28" width="11.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="28" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="28" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="51.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" s="30" t="n">
+        <v>14000</v>
+      </c>
+      <c r="E2" s="30" t="n">
+        <f aca="false">INT(D2/0.2265 )</f>
+        <v>61810</v>
+      </c>
+      <c r="F2" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D3" s="33" t="n">
+        <v>13500</v>
+      </c>
+      <c r="E3" s="33" t="n">
+        <f aca="false">INT(D3/0.2265 )</f>
+        <v>59602</v>
+      </c>
+      <c r="F3" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="36"/>
+      <c r="M3" s="37" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="38" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E4" s="38" t="n">
+        <f aca="false">INT(D4/0.2265 )</f>
+        <v>44150</v>
+      </c>
+      <c r="F4" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="41" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" s="38" t="n">
+        <v>11400</v>
+      </c>
+      <c r="E5" s="38" t="n">
+        <f aca="false">INT(D5/0.2265 )</f>
+        <v>50331</v>
+      </c>
+      <c r="F5" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D6" s="33" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E6" s="33" t="n">
+        <f aca="false">INT(D6/0.2265 )</f>
+        <v>64017</v>
+      </c>
+      <c r="F6" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="43" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" s="33" t="n">
+        <v>10400</v>
+      </c>
+      <c r="E7" s="33" t="n">
+        <f aca="false">INT(D7/0.2265 )</f>
+        <v>45916</v>
+      </c>
+      <c r="F7" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="44" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="33" t="n">
+        <v>12000</v>
+      </c>
+      <c r="E8" s="33" t="n">
+        <f aca="false">INT(D8/0.2265 )</f>
+        <v>52980</v>
+      </c>
+      <c r="F8" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="M8" s="45" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" s="33" t="n">
+        <v>14800</v>
+      </c>
+      <c r="E9" s="33" t="n">
+        <f aca="false">INT(D9/0.2265 )</f>
+        <v>65342</v>
+      </c>
+      <c r="F9" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="D10" s="33" t="n">
+        <v>12000</v>
+      </c>
+      <c r="E10" s="33" t="n">
+        <f aca="false">INT(D10/0.2265 )</f>
+        <v>52980</v>
+      </c>
+      <c r="F10" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="D11" s="33" t="n">
+        <v>11500</v>
+      </c>
+      <c r="E11" s="33" t="n">
+        <f aca="false">INT(D11/0.2265 )</f>
+        <v>50772</v>
+      </c>
+      <c r="F11" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" s="38" t="n">
+        <v>13500</v>
+      </c>
+      <c r="E12" s="38" t="n">
+        <f aca="false">INT(D12/0.2265 )</f>
+        <v>59602</v>
+      </c>
+      <c r="F12" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="40" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="36"/>
+      <c r="K12" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C62,"Resección")</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13" s="33" t="n">
+        <v>11000</v>
+      </c>
+      <c r="E13" s="33" t="n">
+        <f aca="false">INT(D13/0.2265 )</f>
+        <v>48565</v>
+      </c>
+      <c r="F13" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="I13" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C62,"Endoscopia")</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14" s="30" t="n">
+        <v>15500</v>
+      </c>
+      <c r="E14" s="30" t="n">
+        <f aca="false">INT(D14/0.2265 )</f>
+        <v>68432</v>
+      </c>
+      <c r="F14" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" s="32" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="D15" s="30" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E15" s="30" t="n">
+        <f aca="false">INT(D15/0.2265 )</f>
+        <v>66225</v>
+      </c>
+      <c r="F15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C18,"Resección")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="D16" s="38" t="n">
+        <v>9500</v>
+      </c>
+      <c r="E16" s="38" t="n">
+        <f aca="false">INT(D16/0.2265 )</f>
+        <v>41942</v>
+      </c>
+      <c r="F16" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="I16" s="40" t="n">
+        <v>3</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C18,"Endoscopia")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="38" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E17" s="38" t="n">
+        <f aca="false">INT(D17/0.2265 )</f>
+        <v>66225</v>
+      </c>
+      <c r="F17" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="I17" s="40" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="D18" s="38" t="n">
+        <v>15500</v>
+      </c>
+      <c r="E18" s="38" t="n">
+        <f aca="false">INT(D18/0.2265 )</f>
+        <v>68432</v>
+      </c>
+      <c r="F18" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="I18" s="40" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="48"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="51"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>318</v>
+      </c>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="51"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="51"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" s="51"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="51"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" s="51"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>318</v>
+      </c>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" s="51"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" s="51"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" s="51"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" s="51"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>318</v>
+      </c>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" s="51"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>318</v>
+      </c>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" s="51"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I32" s="51"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I33" s="51"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" s="51"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I35" s="51"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I36" s="51"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>318</v>
+      </c>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I37" s="51"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I38" s="51"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50" t="n">
+        <v>3</v>
+      </c>
+      <c r="I39" s="51"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="54"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="54"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="54"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="54"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="54"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="0" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="54"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="54"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="54"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="54"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
+      <c r="F50" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="54"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="54"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="54"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
+      <c r="F53" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="54"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="54"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="54"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="54"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="54"/>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="54"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" s="53"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="54"/>
+      <c r="J59" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="53"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="54"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D61" s="52"/>
+      <c r="E61" s="52"/>
+      <c r="F61" s="53" t="n">
+        <v>2</v>
+      </c>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="54"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C62" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="G62" s="53"/>
+      <c r="H62" s="53"/>
+      <c r="I62" s="54"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Cambios en HER2.xlsx: coordenadas mínimas y tipo de biopsias
</commit_message>
<xml_diff>
--- a/data/extras/ihc_slides/HER2.xlsx
+++ b/data/extras/ihc_slides/HER2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Información original" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="408">
   <si>
     <t xml:space="preserve">Nombre Imagen</t>
   </si>
@@ -1112,6 +1112,12 @@
     <t xml:space="preserve">Tipo de biopsia</t>
   </si>
   <si>
+    <t xml:space="preserve">Coordenada X inicial (μm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordenada X inicial (pixeles)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Patólogo 0</t>
   </si>
   <si>
@@ -1145,12 +1151,24 @@
     <t xml:space="preserve">2 patólogos coinciden, 1 no evalúa</t>
   </si>
   <si>
-    <t xml:space="preserve">2 patólogos disiente, 1 no evalúa</t>
+    <t xml:space="preserve">2 patólogos disienten, 1 no evalúa</t>
   </si>
   <si>
     <t xml:space="preserve">Sólo 1 patólogo evalúa </t>
   </si>
   <si>
+    <t xml:space="preserve"># de resecciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># de endocopias</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># de resecciones con consenso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># de endocopias con consenso</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID Biopsia</t>
   </si>
   <si>
@@ -1374,24 +1392,6 @@
   </si>
   <si>
     <t xml:space="preserve">2009-01-61 MCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordenada X inicial (μm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordenada X inicial (pixeles)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># de resecciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># de endocopias</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># de resecciones con consenso</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># de endocopias con consenso</t>
   </si>
   <si>
     <t xml:space="preserve">o endoscopia?</t>
@@ -1824,7 +1824,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7192,25 +7192,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="36.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="25.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="28" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="28" width="14.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="28" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="28" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="28" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="28" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="51.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7226,14 +7228,20 @@
       <c r="D1" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="20" t="s">
         <v>315</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7244,22 +7252,29 @@
         <v>16</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>316</v>
-      </c>
-      <c r="D2" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="31" t="n">
-        <v>0</v>
+        <v>318</v>
+      </c>
+      <c r="D2" s="30" t="n">
+        <v>14000</v>
+      </c>
+      <c r="E2" s="30" t="n">
+        <f aca="false">INT(D2/0.2265 )</f>
+        <v>61810</v>
       </c>
       <c r="F2" s="31" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>317</v>
+      <c r="G2" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7270,23 +7285,30 @@
         <v>110</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="D3" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="34" t="n">
+        <v>320</v>
+      </c>
+      <c r="D3" s="33" t="n">
+        <v>13500</v>
+      </c>
+      <c r="E3" s="33" t="n">
+        <f aca="false">INT(D3/0.2265 )</f>
+        <v>59602</v>
+      </c>
+      <c r="F3" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37" t="s">
-        <v>319</v>
+      <c r="H3" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="36"/>
+      <c r="M3" s="37" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7297,20 +7319,27 @@
         <v>10</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>318</v>
-      </c>
-      <c r="D4" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="39"/>
+        <v>320</v>
+      </c>
+      <c r="D4" s="38" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E4" s="38" t="n">
+        <f aca="false">INT(D4/0.2265 )</f>
+        <v>44150</v>
+      </c>
       <c r="F4" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="41" t="s">
-        <v>320</v>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="41" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7321,20 +7350,27 @@
         <v>116</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="D5" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="39"/>
+        <v>318</v>
+      </c>
+      <c r="D5" s="38" t="n">
+        <v>11400</v>
+      </c>
+      <c r="E5" s="38" t="n">
+        <f aca="false">INT(D5/0.2265 )</f>
+        <v>50331</v>
+      </c>
       <c r="F5" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="42" t="s">
-        <v>321</v>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7345,22 +7381,29 @@
         <v>92</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="D6" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="34" t="n">
+        <v>320</v>
+      </c>
+      <c r="D6" s="33" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E6" s="33" t="n">
+        <f aca="false">INT(D6/0.2265 )</f>
+        <v>64017</v>
+      </c>
+      <c r="F6" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="34" t="n">
+      <c r="H6" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="35" t="n">
+      <c r="I6" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="43" t="s">
-        <v>322</v>
+      <c r="M6" s="43" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7371,22 +7414,29 @@
         <v>112</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="D7" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="34" t="n">
+        <v>320</v>
+      </c>
+      <c r="D7" s="33" t="n">
+        <v>10400</v>
+      </c>
+      <c r="E7" s="33" t="n">
+        <f aca="false">INT(D7/0.2265 )</f>
+        <v>45916</v>
+      </c>
+      <c r="F7" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="34" t="n">
+      <c r="H7" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="35" t="n">
+      <c r="I7" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="K7" s="44" t="s">
-        <v>323</v>
+      <c r="M7" s="44" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7397,22 +7447,29 @@
         <v>6</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="D8" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="34" t="n">
-        <v>2</v>
+        <v>320</v>
+      </c>
+      <c r="D8" s="33" t="n">
+        <v>12000</v>
+      </c>
+      <c r="E8" s="33" t="n">
+        <f aca="false">INT(D8/0.2265 )</f>
+        <v>52980</v>
       </c>
       <c r="F8" s="34" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" s="45" t="s">
-        <v>324</v>
+        <v>0</v>
+      </c>
+      <c r="G8" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="M8" s="45" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7423,18 +7480,25 @@
         <v>88</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="D9" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="34" t="n">
-        <v>2</v>
+        <v>320</v>
+      </c>
+      <c r="D9" s="33" t="n">
+        <v>14800</v>
+      </c>
+      <c r="E9" s="33" t="n">
+        <f aca="false">INT(D9/0.2265 )</f>
+        <v>65342</v>
       </c>
       <c r="F9" s="34" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="35" t="n">
         <v>2</v>
       </c>
     </row>
@@ -7446,18 +7510,25 @@
         <v>130</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="D10" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="34" t="n">
-        <v>2</v>
+        <v>318</v>
+      </c>
+      <c r="D10" s="33" t="n">
+        <v>12000</v>
+      </c>
+      <c r="E10" s="33" t="n">
+        <f aca="false">INT(D10/0.2265 )</f>
+        <v>52980</v>
       </c>
       <c r="F10" s="34" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="35" t="n">
         <v>2</v>
       </c>
     </row>
@@ -7469,18 +7540,25 @@
         <v>134</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="D11" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="34" t="n">
-        <v>2</v>
+        <v>318</v>
+      </c>
+      <c r="D11" s="33" t="n">
+        <v>11500</v>
+      </c>
+      <c r="E11" s="33" t="n">
+        <f aca="false">INT(D11/0.2265 )</f>
+        <v>50772</v>
       </c>
       <c r="F11" s="34" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="35" t="n">
         <v>2</v>
       </c>
     </row>
@@ -7492,19 +7570,33 @@
         <v>47</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>318</v>
-      </c>
-      <c r="D12" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="39"/>
+        <v>320</v>
+      </c>
+      <c r="D12" s="38" t="n">
+        <v>13500</v>
+      </c>
+      <c r="E12" s="38" t="n">
+        <f aca="false">INT(D12/0.2265 )</f>
+        <v>59602</v>
+      </c>
       <c r="F12" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="40" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" s="36"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="40" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="36"/>
+      <c r="K12" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C62,"Resección")</f>
+        <v>35</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="33" t="s">
@@ -7514,19 +7606,33 @@
         <v>84</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="D13" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="34" t="n">
+        <v>318</v>
+      </c>
+      <c r="D13" s="33" t="n">
+        <v>11000</v>
+      </c>
+      <c r="E13" s="33" t="n">
+        <f aca="false">INT(D13/0.2265 )</f>
+        <v>48565</v>
+      </c>
+      <c r="F13" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="F13" s="34" t="n">
+      <c r="H13" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G13" s="35" t="n">
+      <c r="I13" s="35" t="n">
         <v>3</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C62,"Endoscopia")</f>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7537,18 +7643,25 @@
         <v>49</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="D14" s="31" t="n">
-        <v>3</v>
-      </c>
-      <c r="E14" s="31" t="n">
-        <v>3</v>
+        <v>320</v>
+      </c>
+      <c r="D14" s="30" t="n">
+        <v>15500</v>
+      </c>
+      <c r="E14" s="30" t="n">
+        <f aca="false">INT(D14/0.2265 )</f>
+        <v>68432</v>
       </c>
       <c r="F14" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="G14" s="32" t="n">
+      <c r="G14" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" s="32" t="n">
         <v>3</v>
       </c>
     </row>
@@ -7560,19 +7673,33 @@
         <v>53</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="D15" s="31" t="n">
-        <v>3</v>
-      </c>
-      <c r="E15" s="31" t="n">
-        <v>3</v>
+        <v>320</v>
+      </c>
+      <c r="D15" s="30" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E15" s="30" t="n">
+        <f aca="false">INT(D15/0.2265 )</f>
+        <v>66225</v>
       </c>
       <c r="F15" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="32" t="n">
+      <c r="G15" s="31" t="n">
         <v>3</v>
+      </c>
+      <c r="H15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C18,"Resección")</f>
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7583,17 +7710,31 @@
         <v>55</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="D16" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="E16" s="39"/>
+        <v>318</v>
+      </c>
+      <c r="D16" s="38" t="n">
+        <v>9500</v>
+      </c>
+      <c r="E16" s="38" t="n">
+        <f aca="false">INT(D16/0.2265 )</f>
+        <v>41942</v>
+      </c>
       <c r="F16" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="40" t="n">
+      <c r="G16" s="39"/>
+      <c r="H16" s="39" t="n">
         <v>3</v>
+      </c>
+      <c r="I16" s="40" t="n">
+        <v>3</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C18,"Endoscopia")</f>
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7604,16 +7745,23 @@
         <v>57</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="D17" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="E17" s="39"/>
+        <v>318</v>
+      </c>
+      <c r="D17" s="38" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E17" s="38" t="n">
+        <f aca="false">INT(D17/0.2265 )</f>
+        <v>66225</v>
+      </c>
       <c r="F17" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="G17" s="40" t="n">
+      <c r="G17" s="39"/>
+      <c r="H17" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="I17" s="40" t="n">
         <v>3</v>
       </c>
     </row>
@@ -7625,16 +7773,23 @@
         <v>59</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="D18" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="E18" s="39"/>
+        <v>318</v>
+      </c>
+      <c r="D18" s="38" t="n">
+        <v>15500</v>
+      </c>
+      <c r="E18" s="38" t="n">
+        <f aca="false">INT(D18/0.2265 )</f>
+        <v>68432</v>
+      </c>
       <c r="F18" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="G18" s="40" t="n">
+      <c r="G18" s="39"/>
+      <c r="H18" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="I18" s="40" t="n">
         <v>3</v>
       </c>
     </row>
@@ -7646,18 +7801,20 @@
         <v>124</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>316</v>
-      </c>
-      <c r="D19" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="47" t="n">
+        <v>318</v>
+      </c>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" s="48"/>
+      <c r="H19" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="48"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="49" t="s">
@@ -7667,16 +7824,18 @@
         <v>82</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D20" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
       <c r="F20" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="G20" s="51"/>
+      <c r="I20" s="51"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="49" t="s">
@@ -7686,16 +7845,18 @@
         <v>108</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>318</v>
-      </c>
-      <c r="D21" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="50"/>
+        <v>320</v>
+      </c>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
       <c r="F21" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="51"/>
+      <c r="I21" s="51"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="49" t="s">
@@ -7705,16 +7866,18 @@
         <v>132</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D22" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
       <c r="F22" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="G22" s="51"/>
+      <c r="I22" s="51"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="49" t="s">
@@ -7724,16 +7887,18 @@
         <v>62</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
       <c r="F23" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" s="51"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="49" t="s">
@@ -7743,16 +7908,18 @@
         <v>64</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D24" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
       <c r="F24" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="51"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="49" t="s">
@@ -7762,16 +7929,18 @@
         <v>66</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D25" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
       <c r="F25" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" s="51"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="49" t="s">
@@ -7781,16 +7950,18 @@
         <v>80</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>318</v>
-      </c>
-      <c r="D26" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="50"/>
+        <v>320</v>
+      </c>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
       <c r="F26" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" s="51"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="49" t="s">
@@ -7800,16 +7971,18 @@
         <v>94</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D27" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
       <c r="F27" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G27" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" s="51"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="49" t="s">
@@ -7819,16 +7992,18 @@
         <v>98</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D28" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
       <c r="F28" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" s="51"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="49" t="s">
@@ -7838,16 +8013,18 @@
         <v>100</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D29" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
       <c r="F29" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G29" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" s="51"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="49" t="s">
@@ -7857,16 +8034,18 @@
         <v>104</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>318</v>
-      </c>
-      <c r="D30" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="50"/>
+        <v>320</v>
+      </c>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
       <c r="F30" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G30" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" s="51"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="49" t="s">
@@ -7876,16 +8055,18 @@
         <v>106</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>318</v>
-      </c>
-      <c r="D31" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="50"/>
+        <v>320</v>
+      </c>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
       <c r="F31" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" s="51"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="49" t="s">
@@ -7895,16 +8076,18 @@
         <v>27</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D32" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
       <c r="F32" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I32" s="51"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="49" t="s">
@@ -7914,16 +8097,18 @@
         <v>122</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D33" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
       <c r="F33" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I33" s="51"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="49" t="s">
@@ -7933,16 +8118,18 @@
         <v>126</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D34" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="50"/>
+        <v>318</v>
+      </c>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
       <c r="F34" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G34" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" s="51"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="49" t="s">
@@ -7952,16 +8139,18 @@
         <v>29</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D35" s="50" t="n">
+        <v>318</v>
+      </c>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G35" s="51"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I35" s="51"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="49" t="s">
@@ -7971,16 +8160,18 @@
         <v>31</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D36" s="50" t="n">
+        <v>318</v>
+      </c>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G36" s="51"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I36" s="51"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="49" t="s">
@@ -7990,16 +8181,18 @@
         <v>37</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>318</v>
-      </c>
-      <c r="D37" s="50" t="n">
+        <v>320</v>
+      </c>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G37" s="51"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I37" s="51"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="49" t="s">
@@ -8009,16 +8202,18 @@
         <v>39</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D38" s="50" t="n">
+        <v>318</v>
+      </c>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G38" s="51"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I38" s="51"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="49" t="s">
@@ -8028,16 +8223,18 @@
         <v>35</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>316</v>
-      </c>
-      <c r="D39" s="50" t="n">
+        <v>318</v>
+      </c>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50" t="n">
+      <c r="G39" s="50"/>
+      <c r="H39" s="50" t="n">
         <v>3</v>
       </c>
-      <c r="G39" s="51"/>
+      <c r="I39" s="51"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="52" t="s">
@@ -8047,14 +8244,16 @@
         <v>68</v>
       </c>
       <c r="C40" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D40" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="54"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="52" t="s">
@@ -8064,14 +8263,16 @@
         <v>70</v>
       </c>
       <c r="C41" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D41" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="54"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="52" t="s">
@@ -8081,14 +8282,16 @@
         <v>72</v>
       </c>
       <c r="C42" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D42" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="54"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="52" t="s">
@@ -8098,14 +8301,16 @@
         <v>14</v>
       </c>
       <c r="C43" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D43" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="54"/>
+        <v>320</v>
+      </c>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="54"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="52" t="s">
@@ -8115,14 +8320,16 @@
         <v>19</v>
       </c>
       <c r="C44" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D44" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="54"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="52" t="s">
@@ -8132,14 +8339,16 @@
         <v>74</v>
       </c>
       <c r="C45" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D45" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="54"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="52" t="s">
@@ -8149,14 +8358,16 @@
         <v>76</v>
       </c>
       <c r="C46" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D46" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="54"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="52" t="s">
@@ -8166,14 +8377,16 @@
         <v>78</v>
       </c>
       <c r="C47" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D47" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="54"/>
+        <v>320</v>
+      </c>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="54"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="52" t="s">
@@ -8183,14 +8396,16 @@
         <v>86</v>
       </c>
       <c r="C48" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D48" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="54"/>
+        <v>320</v>
+      </c>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="54"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="52" t="s">
@@ -8200,14 +8415,16 @@
         <v>90</v>
       </c>
       <c r="C49" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D49" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="54"/>
+        <v>320</v>
+      </c>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="54"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="52" t="s">
@@ -8217,14 +8434,16 @@
         <v>96</v>
       </c>
       <c r="C50" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D50" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="54"/>
+        <v>320</v>
+      </c>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
+      <c r="F50" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="54"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="52" t="s">
@@ -8234,14 +8453,16 @@
         <v>102</v>
       </c>
       <c r="C51" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D51" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="54"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="52" t="s">
@@ -8251,14 +8472,16 @@
         <v>23</v>
       </c>
       <c r="C52" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D52" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="54"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="52" t="s">
@@ -8268,14 +8491,16 @@
         <v>114</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D53" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
+      <c r="F53" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="54"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="52" t="s">
@@ -8285,14 +8510,16 @@
         <v>25</v>
       </c>
       <c r="C54" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D54" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="54"/>
+        <v>320</v>
+      </c>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="54"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="52" t="s">
@@ -8302,14 +8529,16 @@
         <v>118</v>
       </c>
       <c r="C55" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D55" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" s="53"/>
-      <c r="F55" s="53"/>
-      <c r="G55" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="54"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="52" t="s">
@@ -8319,14 +8548,16 @@
         <v>120</v>
       </c>
       <c r="C56" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D56" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="54"/>
+        <v>320</v>
+      </c>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="54"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="52" t="s">
@@ -8336,14 +8567,16 @@
         <v>128</v>
       </c>
       <c r="C57" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D57" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" s="53"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="54"/>
+        <v>318</v>
+      </c>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="54"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="52" t="s">
@@ -8353,14 +8586,16 @@
         <v>33</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D58" s="53" t="n">
+        <v>320</v>
+      </c>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="53" t="n">
         <v>1</v>
       </c>
-      <c r="E58" s="53"/>
-      <c r="F58" s="53"/>
-      <c r="G58" s="54"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="54"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="52" t="s">
@@ -8370,14 +8605,16 @@
         <v>41</v>
       </c>
       <c r="C59" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D59" s="53" t="n">
+        <v>320</v>
+      </c>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="53" t="n">
         <v>1</v>
       </c>
-      <c r="E59" s="53"/>
-      <c r="F59" s="53"/>
-      <c r="G59" s="54"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="54"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="52" t="s">
@@ -8387,14 +8624,16 @@
         <v>43</v>
       </c>
       <c r="C60" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D60" s="53" t="n">
+        <v>320</v>
+      </c>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="53" t="n">
         <v>1</v>
       </c>
-      <c r="E60" s="53"/>
-      <c r="F60" s="53"/>
-      <c r="G60" s="54"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="54"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="52" t="s">
@@ -8404,14 +8643,16 @@
         <v>45</v>
       </c>
       <c r="C61" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D61" s="53" t="n">
-        <v>2</v>
-      </c>
-      <c r="E61" s="53"/>
-      <c r="F61" s="53"/>
-      <c r="G61" s="54"/>
+        <v>320</v>
+      </c>
+      <c r="D61" s="52"/>
+      <c r="E61" s="52"/>
+      <c r="F61" s="53" t="n">
+        <v>2</v>
+      </c>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="54"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="52" t="s">
@@ -8421,14 +8662,16 @@
         <v>51</v>
       </c>
       <c r="C62" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D62" s="53" t="n">
+        <v>320</v>
+      </c>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="53" t="n">
         <v>3</v>
       </c>
-      <c r="E62" s="53"/>
-      <c r="F62" s="53"/>
-      <c r="G62" s="54"/>
+      <c r="G62" s="53"/>
+      <c r="H62" s="53"/>
+      <c r="I62" s="54"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
@@ -8469,16 +8712,16 @@
         <v>310</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="F1" s="56" t="s">
         <v>4</v>
@@ -8487,16 +8730,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="57" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D2" s="57" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="E2" s="57" t="s">
         <v>46</v>
@@ -8506,16 +8749,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="57" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B3" s="57" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="E3" s="57" t="s">
         <v>30</v>
@@ -8525,16 +8768,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="57" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="B4" s="57" t="s">
         <v>64</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="E4" s="57" t="s">
         <v>63</v>
@@ -8544,16 +8787,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="57" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="B5" s="57" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D5" s="57" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="E5" s="57" t="s">
         <v>67</v>
@@ -8563,16 +8806,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="57" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B6" s="57" t="s">
         <v>74</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D6" s="57" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="E6" s="57" t="s">
         <v>73</v>
@@ -8582,16 +8825,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="57" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B7" s="57" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D7" s="57" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="E7" s="57" t="s">
         <v>24</v>
@@ -8601,16 +8844,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="57" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B8" s="57" t="s">
         <v>66</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D8" s="57" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="E8" s="57" t="s">
         <v>65</v>
@@ -8620,16 +8863,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="57" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B9" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="E9" s="57" t="s">
         <v>22</v>
@@ -8639,16 +8882,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="57" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="B10" s="57" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D10" s="57" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="E10" s="57" t="s">
         <v>32</v>
@@ -8658,16 +8901,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="57" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="B11" s="57" t="s">
         <v>128</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D11" s="57" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="E11" s="57" t="s">
         <v>127</v>
@@ -8677,13 +8920,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="57" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="B12" s="57" t="s">
         <v>110</v>
       </c>
       <c r="C12" s="57" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D12" s="57" t="n">
         <v>102974</v>
@@ -8696,16 +8939,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="57" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="B13" s="57" t="s">
         <v>70</v>
       </c>
       <c r="C13" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D13" s="57" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="E13" s="57" t="s">
         <v>69</v>
@@ -8715,37 +8958,37 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="58" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="B14" s="58" t="s">
         <v>57</v>
       </c>
       <c r="C14" s="58" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D14" s="58" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="E14" s="58" t="s">
         <v>56</v>
       </c>
       <c r="F14" s="58" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="G14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="57" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B15" s="57" t="s">
         <v>100</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="E15" s="57" t="s">
         <v>99</v>
@@ -8755,16 +8998,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="57" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B16" s="57" t="s">
         <v>122</v>
       </c>
       <c r="C16" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D16" s="57" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="E16" s="57" t="s">
         <v>121</v>
@@ -8774,16 +9017,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="57" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B17" s="57" t="s">
         <v>108</v>
       </c>
       <c r="C17" s="57" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D17" s="57" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="E17" s="57" t="s">
         <v>107</v>
@@ -8793,16 +9036,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="57" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="B18" s="57" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D18" s="57" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="E18" s="57" t="s">
         <v>13</v>
@@ -8812,16 +9055,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="57" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="B19" s="57" t="s">
         <v>124</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D19" s="57" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="E19" s="57" t="s">
         <v>123</v>
@@ -8831,16 +9074,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="57" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B20" s="57" t="s">
         <v>78</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="E20" s="57" t="s">
         <v>77</v>
@@ -8850,16 +9093,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="57" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B21" s="57" t="s">
         <v>114</v>
       </c>
       <c r="C21" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D21" s="57" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="E21" s="57" t="s">
         <v>113</v>
@@ -8869,37 +9112,37 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="58" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B22" s="58" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="E22" s="58" t="s">
         <v>44</v>
       </c>
       <c r="F22" s="58" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="G22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="57" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B23" s="57" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D23" s="57" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="E23" s="57" t="s">
         <v>28</v>
@@ -8909,16 +9152,16 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="57" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="B24" s="57" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D24" s="57" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="E24" s="57" t="s">
         <v>15</v>
@@ -8928,16 +9171,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="57" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="B25" s="57" t="s">
         <v>84</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D25" s="57" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="E25" s="57" t="s">
         <v>83</v>
@@ -8947,7 +9190,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="59" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="B26" s="59" t="s">
         <v>72</v>
@@ -8958,22 +9201,22 @@
         <v>71</v>
       </c>
       <c r="F26" s="59" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="G26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="57" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="B27" s="57" t="s">
         <v>104</v>
       </c>
       <c r="C27" s="57" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="E27" s="57" t="s">
         <v>103</v>
@@ -8983,7 +9226,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="59" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="B28" s="59" t="s">
         <v>88</v>
@@ -8994,55 +9237,55 @@
         <v>87</v>
       </c>
       <c r="F28" s="59" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="G28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="58" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B29" s="58" t="s">
         <v>134</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="E29" s="58" t="s">
         <v>133</v>
       </c>
       <c r="F29" s="58" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="G29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="58" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B30" s="58" t="s">
         <v>92</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="E30" s="58" t="s">
         <v>91</v>
       </c>
       <c r="F30" s="58" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="G30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="59" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B31" s="59" t="s">
         <v>43</v>
@@ -9057,7 +9300,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="59" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B32" s="59" t="s">
         <v>76</v>
@@ -9072,7 +9315,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="59" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B33" s="59" t="s">
         <v>96</v>
@@ -9087,7 +9330,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="59" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="B34" s="59" t="s">
         <v>132</v>
@@ -9102,7 +9345,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="59" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B35" s="59" t="s">
         <v>86</v>
@@ -9117,7 +9360,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="59" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B36" s="59" t="s">
         <v>62</v>
@@ -9132,7 +9375,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="59" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="B37" s="59" t="s">
         <v>112</v>
@@ -9147,7 +9390,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="59" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="B38" s="59" t="s">
         <v>59</v>
@@ -9162,7 +9405,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="59" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="B39" s="59" t="s">
         <v>53</v>
@@ -9177,7 +9420,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="59" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="B40" s="59" t="s">
         <v>130</v>
@@ -9192,7 +9435,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="59" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="B41" s="59" t="s">
         <v>118</v>
@@ -9207,7 +9450,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="59" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B42" s="59" t="s">
         <v>27</v>
@@ -9222,7 +9465,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="59" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B43" s="59" t="s">
         <v>120</v>
@@ -9237,7 +9480,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="59" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B44" s="59" t="s">
         <v>106</v>
@@ -9252,7 +9495,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="59" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B45" s="59" t="s">
         <v>126</v>
@@ -9267,7 +9510,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="59" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="B46" s="59" t="s">
         <v>116</v>
@@ -9282,7 +9525,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="59" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B47" s="59" t="s">
         <v>39</v>
@@ -9297,7 +9540,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="59" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B48" s="59" t="s">
         <v>80</v>
@@ -9312,7 +9555,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="59" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B49" s="59" t="s">
         <v>55</v>
@@ -9327,7 +9570,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="59" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B50" s="59" t="s">
         <v>51</v>
@@ -9342,7 +9585,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="59" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="B51" s="59" t="s">
         <v>90</v>
@@ -9357,7 +9600,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="59" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="B52" s="59" t="s">
         <v>98</v>
@@ -9372,7 +9615,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="59" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="B53" s="59" t="s">
         <v>102</v>
@@ -9387,7 +9630,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="59" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="B54" s="59" t="s">
         <v>10</v>
@@ -9402,7 +9645,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="59" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="B55" s="59" t="s">
         <v>82</v>
@@ -9417,7 +9660,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="59" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="B56" s="59" t="s">
         <v>6</v>
@@ -9432,7 +9675,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="59" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="B57" s="59" t="s">
         <v>35</v>
@@ -9447,7 +9690,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="59" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B58" s="59" t="s">
         <v>94</v>
@@ -9462,7 +9705,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="59" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="B59" s="59" t="s">
         <v>49</v>
@@ -9477,7 +9720,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="59" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="B60" s="59" t="s">
         <v>37</v>
@@ -9492,7 +9735,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="59" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="B61" s="59" t="s">
         <v>41</v>
@@ -9507,7 +9750,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="59" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="B62" s="59" t="s">
         <v>19</v>
@@ -9539,8 +9782,8 @@
   </sheetPr>
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9572,22 +9815,22 @@
         <v>311</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>400</v>
+        <v>312</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>401</v>
+        <v>313</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9598,7 +9841,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D2" s="30" t="n">
         <v>14000</v>
@@ -9620,7 +9863,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9631,7 +9874,7 @@
         <v>110</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D3" s="33" t="n">
         <v>13500</v>
@@ -9654,7 +9897,7 @@
       </c>
       <c r="L3" s="36"/>
       <c r="M3" s="37" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9665,7 +9908,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D4" s="38" t="n">
         <v>10000</v>
@@ -9685,7 +9928,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="41" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9696,7 +9939,7 @@
         <v>116</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D5" s="38" t="n">
         <v>11400</v>
@@ -9716,7 +9959,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="42" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9727,7 +9970,7 @@
         <v>92</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D6" s="33" t="n">
         <v>14500</v>
@@ -9749,7 +9992,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="43" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9760,7 +10003,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D7" s="33" t="n">
         <v>10400</v>
@@ -9782,7 +10025,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="44" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9793,7 +10036,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D8" s="33" t="n">
         <v>12000</v>
@@ -9815,7 +10058,7 @@
         <v>2</v>
       </c>
       <c r="M8" s="45" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9826,7 +10069,7 @@
         <v>88</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D9" s="33" t="n">
         <v>14800</v>
@@ -9856,7 +10099,7 @@
         <v>130</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D10" s="33" t="n">
         <v>12000</v>
@@ -9886,7 +10129,7 @@
         <v>134</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D11" s="33" t="n">
         <v>11500</v>
@@ -9916,7 +10159,7 @@
         <v>47</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D12" s="38" t="n">
         <v>13500</v>
@@ -9937,7 +10180,7 @@
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="0" t="s">
-        <v>402</v>
+        <v>327</v>
       </c>
       <c r="L12" s="0" t="n">
         <f aca="false">COUNTIF(C2:C62,"Resección")</f>
@@ -9952,7 +10195,7 @@
         <v>84</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D13" s="33" t="n">
         <v>11000</v>
@@ -9974,7 +10217,7 @@
         <v>3</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>403</v>
+        <v>328</v>
       </c>
       <c r="L13" s="0" t="n">
         <f aca="false">COUNTIF(C2:C62,"Endoscopia")</f>
@@ -9989,7 +10232,7 @@
         <v>49</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D14" s="30" t="n">
         <v>15500</v>
@@ -10019,7 +10262,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D15" s="30" t="n">
         <v>15000</v>
@@ -10041,7 +10284,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>404</v>
+        <v>329</v>
       </c>
       <c r="L15" s="0" t="n">
         <f aca="false">COUNTIF(C2:C18,"Resección")</f>
@@ -10056,7 +10299,7 @@
         <v>55</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D16" s="38" t="n">
         <v>9500</v>
@@ -10076,7 +10319,7 @@
         <v>3</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>405</v>
+        <v>330</v>
       </c>
       <c r="L16" s="0" t="n">
         <f aca="false">COUNTIF(C2:C18,"Endoscopia")</f>
@@ -10091,7 +10334,7 @@
         <v>57</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D17" s="38" t="n">
         <v>15000</v>
@@ -10119,7 +10362,7 @@
         <v>59</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D18" s="38" t="n">
         <v>15500</v>
@@ -10147,7 +10390,7 @@
         <v>124</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D19" s="46"/>
       <c r="E19" s="46"/>
@@ -10170,7 +10413,7 @@
         <v>82</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="49"/>
@@ -10191,7 +10434,7 @@
         <v>108</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="49"/>
@@ -10212,7 +10455,7 @@
         <v>132</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="49"/>
@@ -10233,7 +10476,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="49"/>
@@ -10254,7 +10497,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D24" s="49"/>
       <c r="E24" s="49"/>
@@ -10275,7 +10518,7 @@
         <v>66</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D25" s="49"/>
       <c r="E25" s="49"/>
@@ -10296,7 +10539,7 @@
         <v>80</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D26" s="49"/>
       <c r="E26" s="49"/>
@@ -10317,7 +10560,7 @@
         <v>94</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D27" s="49"/>
       <c r="E27" s="49"/>
@@ -10338,7 +10581,7 @@
         <v>98</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D28" s="49"/>
       <c r="E28" s="49"/>
@@ -10359,7 +10602,7 @@
         <v>100</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D29" s="49"/>
       <c r="E29" s="49"/>
@@ -10380,7 +10623,7 @@
         <v>104</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D30" s="49"/>
       <c r="E30" s="49"/>
@@ -10401,7 +10644,7 @@
         <v>106</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D31" s="49"/>
       <c r="E31" s="49"/>
@@ -10422,7 +10665,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D32" s="49"/>
       <c r="E32" s="49"/>
@@ -10443,7 +10686,7 @@
         <v>122</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D33" s="49"/>
       <c r="E33" s="49"/>
@@ -10464,7 +10707,7 @@
         <v>126</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D34" s="49"/>
       <c r="E34" s="49"/>
@@ -10485,7 +10728,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D35" s="49"/>
       <c r="E35" s="49"/>
@@ -10506,7 +10749,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D36" s="49"/>
       <c r="E36" s="49"/>
@@ -10527,7 +10770,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D37" s="49"/>
       <c r="E37" s="49"/>
@@ -10548,7 +10791,7 @@
         <v>39</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D38" s="49"/>
       <c r="E38" s="49"/>
@@ -10569,7 +10812,7 @@
         <v>35</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D39" s="49"/>
       <c r="E39" s="49"/>
@@ -10590,7 +10833,7 @@
         <v>68</v>
       </c>
       <c r="C40" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D40" s="52"/>
       <c r="E40" s="52"/>
@@ -10609,7 +10852,7 @@
         <v>70</v>
       </c>
       <c r="C41" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D41" s="52"/>
       <c r="E41" s="52"/>
@@ -10628,7 +10871,7 @@
         <v>72</v>
       </c>
       <c r="C42" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D42" s="52"/>
       <c r="E42" s="52"/>
@@ -10647,7 +10890,7 @@
         <v>14</v>
       </c>
       <c r="C43" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D43" s="52"/>
       <c r="E43" s="52"/>
@@ -10666,7 +10909,7 @@
         <v>19</v>
       </c>
       <c r="C44" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D44" s="52"/>
       <c r="E44" s="52"/>
@@ -10685,7 +10928,7 @@
         <v>74</v>
       </c>
       <c r="C45" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D45" s="52"/>
       <c r="E45" s="52"/>
@@ -10707,7 +10950,7 @@
         <v>76</v>
       </c>
       <c r="C46" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D46" s="52"/>
       <c r="E46" s="52"/>
@@ -10726,7 +10969,7 @@
         <v>78</v>
       </c>
       <c r="C47" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D47" s="52"/>
       <c r="E47" s="52"/>
@@ -10745,7 +10988,7 @@
         <v>86</v>
       </c>
       <c r="C48" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D48" s="52"/>
       <c r="E48" s="52"/>
@@ -10764,7 +11007,7 @@
         <v>90</v>
       </c>
       <c r="C49" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D49" s="52"/>
       <c r="E49" s="52"/>
@@ -10783,7 +11026,7 @@
         <v>96</v>
       </c>
       <c r="C50" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D50" s="52"/>
       <c r="E50" s="52"/>
@@ -10802,7 +11045,7 @@
         <v>102</v>
       </c>
       <c r="C51" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D51" s="52"/>
       <c r="E51" s="52"/>
@@ -10821,7 +11064,7 @@
         <v>23</v>
       </c>
       <c r="C52" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D52" s="52"/>
       <c r="E52" s="52"/>
@@ -10840,7 +11083,7 @@
         <v>114</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D53" s="52"/>
       <c r="E53" s="52"/>
@@ -10859,7 +11102,7 @@
         <v>25</v>
       </c>
       <c r="C54" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D54" s="52"/>
       <c r="E54" s="52"/>
@@ -10878,7 +11121,7 @@
         <v>118</v>
       </c>
       <c r="C55" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D55" s="52"/>
       <c r="E55" s="52"/>
@@ -10897,7 +11140,7 @@
         <v>120</v>
       </c>
       <c r="C56" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D56" s="52"/>
       <c r="E56" s="52"/>
@@ -10916,7 +11159,7 @@
         <v>128</v>
       </c>
       <c r="C57" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D57" s="52"/>
       <c r="E57" s="52"/>
@@ -10935,7 +11178,7 @@
         <v>33</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D58" s="52"/>
       <c r="E58" s="52"/>
@@ -10954,7 +11197,7 @@
         <v>41</v>
       </c>
       <c r="C59" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D59" s="52"/>
       <c r="E59" s="52"/>
@@ -10976,7 +11219,7 @@
         <v>43</v>
       </c>
       <c r="C60" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D60" s="52"/>
       <c r="E60" s="52"/>
@@ -10995,7 +11238,7 @@
         <v>45</v>
       </c>
       <c r="C61" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D61" s="52"/>
       <c r="E61" s="52"/>
@@ -11014,7 +11257,7 @@
         <v>51</v>
       </c>
       <c r="C62" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D62" s="52"/>
       <c r="E62" s="52"/>

</xml_diff>